<commit_message>
Minor updates, added some data to Habitat_Raw
</commit_message>
<xml_diff>
--- a/Output/Habitat_Attributes_Ratings_Table.xlsx
+++ b/Output/Habitat_Attributes_Ratings_Table.xlsx
@@ -33010,7 +33010,12 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>Adequate</t>
+          <t>At Risk</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>At Risk</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -33122,7 +33127,12 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>Adequate</t>
+          <t>At Risk</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>At Risk</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -65942,7 +65952,7 @@
       </c>
       <c r="E547" t="inlineStr">
         <is>
-          <t>Adequate</t>
+          <t>Unacceptable</t>
         </is>
       </c>
       <c r="F547" t="inlineStr">
@@ -65962,7 +65972,7 @@
       </c>
       <c r="I547" t="inlineStr">
         <is>
-          <t>Adequate</t>
+          <t>At Risk</t>
         </is>
       </c>
       <c r="J547" t="inlineStr">
@@ -73070,7 +73080,7 @@
       </c>
       <c r="E601" t="inlineStr">
         <is>
-          <t>At Risk</t>
+          <t>Unacceptable</t>
         </is>
       </c>
       <c r="F601" t="inlineStr">
@@ -73078,14 +73088,44 @@
           <t>Unacceptable</t>
         </is>
       </c>
+      <c r="G601" t="inlineStr">
+        <is>
+          <t>Unacceptable</t>
+        </is>
+      </c>
+      <c r="H601" t="inlineStr">
+        <is>
+          <t>Unacceptable</t>
+        </is>
+      </c>
+      <c r="I601" t="inlineStr">
+        <is>
+          <t>Unacceptable</t>
+        </is>
+      </c>
+      <c r="J601" t="inlineStr">
+        <is>
+          <t>Unacceptable</t>
+        </is>
+      </c>
       <c r="K601" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>Unacceptable</t>
+        </is>
+      </c>
+      <c r="L601" t="inlineStr">
+        <is>
+          <t>At Risk</t>
+        </is>
+      </c>
+      <c r="M601" t="inlineStr">
+        <is>
+          <t>Unacceptable</t>
         </is>
       </c>
       <c r="N601" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>At Risk</t>
         </is>
       </c>
       <c r="O601" t="inlineStr">
@@ -73103,11 +73143,6 @@
           <t>Adequate</t>
         </is>
       </c>
-      <c r="R601" t="inlineStr">
-        <is>
-          <t>Adequate</t>
-        </is>
-      </c>
       <c r="S601" t="inlineStr">
         <is>
           <t>Adequate</t>
@@ -73154,11 +73189,6 @@
         </is>
       </c>
       <c r="AB601" t="inlineStr">
-        <is>
-          <t>Adequate</t>
-        </is>
-      </c>
-      <c r="AC601" t="inlineStr">
         <is>
           <t>Adequate</t>
         </is>
@@ -73197,6 +73227,11 @@
       </c>
       <c r="F602" t="inlineStr">
         <is>
+          <t>Unacceptable</t>
+        </is>
+      </c>
+      <c r="G602" t="inlineStr">
+        <is>
           <t>Adequate</t>
         </is>
       </c>
@@ -73210,14 +73245,29 @@
           <t>At Risk</t>
         </is>
       </c>
+      <c r="J602" t="inlineStr">
+        <is>
+          <t>Adequate</t>
+        </is>
+      </c>
       <c r="K602" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>Adequate</t>
+        </is>
+      </c>
+      <c r="L602" t="inlineStr">
+        <is>
+          <t>Adequate</t>
+        </is>
+      </c>
+      <c r="M602" t="inlineStr">
+        <is>
+          <t>At Risk</t>
         </is>
       </c>
       <c r="N602" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>At Risk</t>
         </is>
       </c>
       <c r="O602" t="inlineStr">
@@ -73286,11 +73336,6 @@
         </is>
       </c>
       <c r="AB602" t="inlineStr">
-        <is>
-          <t>Adequate</t>
-        </is>
-      </c>
-      <c r="AC602" t="inlineStr">
         <is>
           <t>Adequate</t>
         </is>
@@ -73322,19 +73367,54 @@
           <t>Adequate</t>
         </is>
       </c>
+      <c r="E603" t="inlineStr">
+        <is>
+          <t>Adequate</t>
+        </is>
+      </c>
       <c r="F603" t="inlineStr">
         <is>
+          <t>Unacceptable</t>
+        </is>
+      </c>
+      <c r="G603" t="inlineStr">
+        <is>
+          <t>Adequate</t>
+        </is>
+      </c>
+      <c r="H603" t="inlineStr">
+        <is>
+          <t>Adequate</t>
+        </is>
+      </c>
+      <c r="I603" t="inlineStr">
+        <is>
+          <t>Adequate</t>
+        </is>
+      </c>
+      <c r="J603" t="inlineStr">
+        <is>
           <t>Adequate</t>
         </is>
       </c>
       <c r="K603" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>Adequate</t>
+        </is>
+      </c>
+      <c r="L603" t="inlineStr">
+        <is>
+          <t>Adequate</t>
+        </is>
+      </c>
+      <c r="M603" t="inlineStr">
+        <is>
+          <t>Adequate</t>
         </is>
       </c>
       <c r="N603" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>Adequate</t>
         </is>
       </c>
       <c r="O603" t="inlineStr">
@@ -73352,11 +73432,6 @@
           <t>Adequate</t>
         </is>
       </c>
-      <c r="R603" t="inlineStr">
-        <is>
-          <t>Adequate</t>
-        </is>
-      </c>
       <c r="S603" t="inlineStr">
         <is>
           <t>Adequate</t>
@@ -73403,11 +73478,6 @@
         </is>
       </c>
       <c r="AB603" t="inlineStr">
-        <is>
-          <t>Adequate</t>
-        </is>
-      </c>
-      <c r="AC603" t="inlineStr">
         <is>
           <t>Adequate</t>
         </is>

</xml_diff>